<commit_message>
Adding Excel file to Read data
</commit_message>
<xml_diff>
--- a/FindingHospitals_Practo/ReadExcelData.xlsx
+++ b/FindingHospitals_Practo/ReadExcelData.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rupesh\eclipse-workspace\FindingHospitals_Practo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="2625"/>
   </bookViews>
   <sheets>
     <sheet name="ReadData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Rupesh</t>
   </si>
   <si>
-    <t>prosthatic ltd</t>
+    <t>Prosthatic pvt ltd</t>
   </si>
   <si>
     <t>kumar.rex@gmail</t>
@@ -41,7 +37,10 @@
     <t>kumar.rex@gmail.com</t>
   </si>
   <si>
-    <t>98765+21</t>
+    <t>987654+908</t>
+  </si>
+  <si>
+    <t>"9087654321"</t>
   </si>
 </sst>
 </file>
@@ -86,9 +85,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -373,17 +375,17 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="8" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -396,8 +398,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>9876543210</v>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -415,5 +417,6 @@
     <hyperlink ref="F1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>